<commit_message>
regjistri permirsim i njesive
</commit_message>
<xml_diff>
--- a/5-Njësite-banesore/regjistri/16-Regjistri-për-ndërtesë-me-pjesë-të-ndërtesës-2602-0-Albnori.xlsx
+++ b/5-Njësite-banesore/regjistri/16-Regjistri-për-ndërtesë-me-pjesë-të-ndërtesës-2602-0-Albnori.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
   <si>
     <t>Nr</t>
   </si>
@@ -229,9 +229,6 @@
     <t>Ferizaj</t>
   </si>
   <si>
-    <t>N    D    Ë    R    T    E    S    A                    O-72217092-00565-6-385-0</t>
-  </si>
-  <si>
     <t>Gjeodeti apo kompania gjeodete e licencuar: SEAD PRUSHI numri i licencës: 152</t>
   </si>
   <si>
@@ -275,6 +272,24 @@
   </si>
   <si>
     <t>O-72217092-02602-0-_____-0-1-4-0    </t>
+  </si>
+  <si>
+    <t>Depo</t>
+  </si>
+  <si>
+    <t>O-72217092-02602-0-_____-0-1-5-0    </t>
+  </si>
+  <si>
+    <t>N    D    Ë    R    T    E    S    A                    O-72217092-02602-0-______</t>
+  </si>
+  <si>
+    <t>O-72217092-02602-0-_____-0-1-6-0    </t>
+  </si>
+  <si>
+    <t>O-72217092-02602-0-_____-0-1-7-0    </t>
+  </si>
+  <si>
+    <t>O-72217092-02602-0-_____-0-1-8-0    </t>
   </si>
 </sst>
 </file>
@@ -884,7 +899,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -978,6 +993,78 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1059,77 +1146,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1506,10 +1524,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q29"/>
+  <dimension ref="B1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23:I23"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C1" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1532,244 +1550,244 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="35"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="59"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="38"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="62"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="38"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="62"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="38"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="62"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="38"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="62"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="38"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="61"/>
+      <c r="P6" s="61"/>
+      <c r="Q6" s="62"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="36"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="38"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="61"/>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="62"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="38"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="61"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="62"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="36"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="38"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="62"/>
     </row>
     <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="39"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="41"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="64"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="64"/>
+      <c r="P10" s="64"/>
+      <c r="Q10" s="65"/>
     </row>
     <row r="11" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="44"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="67"/>
+      <c r="P11" s="67"/>
+      <c r="Q11" s="68"/>
     </row>
     <row r="12" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="47"/>
+      <c r="B12" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="70"/>
+      <c r="N12" s="70"/>
+      <c r="O12" s="70"/>
+      <c r="P12" s="70"/>
+      <c r="Q12" s="71"/>
     </row>
     <row r="13" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="48"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="49"/>
-      <c r="P13" s="49"/>
-      <c r="Q13" s="50"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="73"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="74"/>
     </row>
     <row r="14" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
@@ -1784,18 +1802,18 @@
       <c r="E14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="60" t="s">
+      <c r="F14" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60" t="s">
+      <c r="G14" s="33"/>
+      <c r="H14" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="60"/>
-      <c r="J14" s="80" t="s">
+      <c r="I14" s="33"/>
+      <c r="J14" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="81"/>
+      <c r="K14" s="40"/>
       <c r="L14" s="11" t="s">
         <v>17</v>
       </c>
@@ -1826,96 +1844,96 @@
         <v>27</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="75">
+        <v>37</v>
+      </c>
+      <c r="F15" s="34">
         <v>125.2</v>
       </c>
-      <c r="G15" s="75"/>
-      <c r="H15" s="76" t="s">
+      <c r="G15" s="34"/>
+      <c r="H15" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="76"/>
-      <c r="J15" s="82" t="s">
+      <c r="I15" s="35"/>
+      <c r="J15" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" s="42"/>
+      <c r="L15" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K15" s="83"/>
-      <c r="L15" s="14" t="s">
-        <v>37</v>
-      </c>
       <c r="M15" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="N15" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="N15" s="14" t="s">
-        <v>35</v>
       </c>
       <c r="O15" s="17">
         <v>1233339128</v>
       </c>
       <c r="P15" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q15" s="19" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="77"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="78"/>
-      <c r="M16" s="78"/>
-      <c r="N16" s="78"/>
-      <c r="O16" s="78"/>
-      <c r="P16" s="78"/>
-      <c r="Q16" s="79"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="38"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="58"/>
-      <c r="L17" s="58"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="58"/>
-      <c r="O17" s="58"/>
-      <c r="P17" s="58"/>
-      <c r="Q17" s="59"/>
+      <c r="B17" s="81" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="82"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="82"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="82"/>
+      <c r="O17" s="82"/>
+      <c r="P17" s="82"/>
+      <c r="Q17" s="83"/>
     </row>
     <row r="18" spans="2:17" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="72" t="s">
+      <c r="C18" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="73"/>
-      <c r="E18" s="74"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="31" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="64" t="s">
+      <c r="H18" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="65"/>
+      <c r="I18" s="47"/>
       <c r="J18" s="31" t="s">
         <v>6</v>
       </c>
@@ -1945,35 +1963,35 @@
       <c r="B19" s="25">
         <v>1</v>
       </c>
-      <c r="C19" s="54" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
+      <c r="C19" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="79"/>
+      <c r="E19" s="80"/>
       <c r="F19" s="26">
         <v>1</v>
       </c>
       <c r="G19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="66">
-        <v>118.31</v>
-      </c>
-      <c r="I19" s="67"/>
+      <c r="H19" s="48">
+        <v>16.27</v>
+      </c>
+      <c r="I19" s="49"/>
       <c r="J19" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="L19" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="K19" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="L19" s="26" t="s">
-        <v>37</v>
-      </c>
       <c r="M19" s="27" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="N19" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O19" s="26">
         <v>1233339128</v>
@@ -1982,42 +2000,40 @@
         <v>8</v>
       </c>
       <c r="Q19" s="29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="5">
-        <v>2</v>
-      </c>
-      <c r="C20" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="25"/>
+      <c r="C20" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="79"/>
+      <c r="E20" s="80"/>
       <c r="F20" s="26">
         <v>1</v>
       </c>
-      <c r="G20" s="2">
-        <v>1</v>
-      </c>
-      <c r="H20" s="66">
-        <v>118.31</v>
-      </c>
-      <c r="I20" s="67"/>
+      <c r="G20" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="48">
+        <v>29.95</v>
+      </c>
+      <c r="I20" s="49"/>
       <c r="J20" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="K20" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="L20" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>33</v>
+      <c r="M20" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="N20" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O20" s="26">
         <v>1233339128</v>
@@ -2026,42 +2042,40 @@
         <v>8</v>
       </c>
       <c r="Q20" s="29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="25">
-        <v>3</v>
-      </c>
-      <c r="C21" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="55"/>
-      <c r="E21" s="56"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="25"/>
+      <c r="C21" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="79"/>
+      <c r="E21" s="80"/>
       <c r="F21" s="26">
         <v>1</v>
       </c>
-      <c r="G21" s="2">
-        <v>2</v>
-      </c>
-      <c r="H21" s="66">
-        <v>118.31</v>
-      </c>
-      <c r="I21" s="67"/>
+      <c r="G21" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="48">
+        <v>65.33</v>
+      </c>
+      <c r="I21" s="49"/>
       <c r="J21" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="L21" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="K21" s="26" t="s">
+      <c r="M21" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="L21" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="N21" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O21" s="26">
         <v>1233339128</v>
@@ -2070,42 +2084,42 @@
         <v>8</v>
       </c>
       <c r="Q21" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="25">
-        <v>7</v>
-      </c>
-      <c r="C22" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="55"/>
-      <c r="E22" s="56"/>
+      <c r="B22" s="5">
+        <v>2</v>
+      </c>
+      <c r="C22" s="78" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="79"/>
+      <c r="E22" s="80"/>
       <c r="F22" s="26">
         <v>1</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
+      <c r="H22" s="48">
+        <v>118.41</v>
+      </c>
+      <c r="I22" s="49"/>
+      <c r="J22" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K22" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="M22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="66">
-        <v>127.2</v>
-      </c>
-      <c r="I22" s="67"/>
-      <c r="J22" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="K22" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="L22" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="N22" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O22" s="26">
         <v>1233339128</v>
@@ -2114,136 +2128,312 @@
         <v>8</v>
       </c>
       <c r="Q22" s="29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="70"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="6"/>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="6"/>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="70"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="6"/>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="6"/>
-    </row>
-    <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="20"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="69"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="23"/>
-      <c r="Q27" s="24"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="84"/>
+      <c r="C23" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="79"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="26">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="48">
+        <v>9.98</v>
+      </c>
+      <c r="I23" s="49"/>
+      <c r="J23" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K23" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="L23" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N23" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="O23" s="26">
+        <v>1233339128</v>
+      </c>
+      <c r="P23" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q23" s="29"/>
+    </row>
+    <row r="24" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="84"/>
+      <c r="C24" s="78" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="79"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="26">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2">
+        <v>2</v>
+      </c>
+      <c r="H24" s="48">
+        <v>118.41</v>
+      </c>
+      <c r="I24" s="49"/>
+      <c r="J24" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K24" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="L24" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N24" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="O24" s="26">
+        <v>1233339128</v>
+      </c>
+      <c r="P24" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q24" s="29"/>
+    </row>
+    <row r="25" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="25">
+        <v>3</v>
+      </c>
+      <c r="C25" s="78" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="79"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="26">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2">
+        <v>2</v>
+      </c>
+      <c r="H25" s="48">
+        <v>9.98</v>
+      </c>
+      <c r="I25" s="49"/>
+      <c r="J25" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K25" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="L25" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N25" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="O25" s="26">
+        <v>1233339128</v>
+      </c>
+      <c r="P25" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q25" s="29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="25">
+        <v>7</v>
+      </c>
+      <c r="C26" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="79"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="26">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" s="48">
+        <v>127.2</v>
+      </c>
+      <c r="I26" s="49"/>
+      <c r="J26" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K26" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="L26" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N26" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="O26" s="26">
+        <v>1233339128</v>
+      </c>
+      <c r="P26" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q26" s="29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="6"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="77"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="6"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="L29" s="7"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="6"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="6"/>
+    </row>
+    <row r="31" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="20"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="23"/>
+      <c r="Q31" s="24"/>
+    </row>
+    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L33" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="40">
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B1:Q10"/>
+    <mergeCell ref="B11:Q11"/>
+    <mergeCell ref="B12:Q12"/>
+    <mergeCell ref="B13:Q13"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="B17:Q17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="H23:I23"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="B16:Q16"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="J15:K15"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="B1:Q10"/>
-    <mergeCell ref="B11:Q11"/>
-    <mergeCell ref="B12:Q12"/>
-    <mergeCell ref="B13:Q13"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="B17:Q17"/>
-    <mergeCell ref="F14:G14"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>